<commit_message>
improved dialog system, can now fulfill a "trade" with the altar
</commit_message>
<xml_diff>
--- a/MiningPrototype/Assets/Other/Dialogs.xlsx
+++ b/MiningPrototype/Assets/Other/Dialogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\BAMiningPrototype\MiningPrototype\Assets\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C0C532-C9D1-48DA-B754-B0B816A22ECF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58263BCF-8BD9-4B4A-9069-E5FC853694B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="1290" windowWidth="24615" windowHeight="13200" xr2:uid="{9FC08946-78F8-47A0-9C11-D535183429CD}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{9FC08946-78F8-47A0-9C11-D535183429CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>SectionName</t>
   </si>
@@ -66,18 +66,6 @@
     <t>Choices4</t>
   </si>
   <si>
-    <t>Choices5</t>
-  </si>
-  <si>
-    <t>Choices6</t>
-  </si>
-  <si>
-    <t>Choices7</t>
-  </si>
-  <si>
-    <t>Choices8</t>
-  </si>
-  <si>
     <t>ChoiceType</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
     <t>Test1_0</t>
   </si>
   <si>
-    <t>Test1_02</t>
-  </si>
-  <si>
     <t>Test1_03</t>
   </si>
   <si>
@@ -126,9 +111,6 @@
     <t>Nothing</t>
   </si>
   <si>
-    <t>Who are you?</t>
-  </si>
-  <si>
     <t>Wealth</t>
   </si>
   <si>
@@ -147,18 +129,6 @@
     <t>and how will you pay?</t>
   </si>
   <si>
-    <t>Test1_021</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Test1_022</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Test1_071</t>
   </si>
   <si>
@@ -177,19 +147,31 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>clear your mind...</t>
-  </si>
-  <si>
     <t>does it look like I need more rocks?</t>
   </si>
   <si>
-    <t>{Amount} {Resource} is the price</t>
-  </si>
-  <si>
-    <t>{Amount} {Resource} will suffice</t>
-  </si>
-  <si>
-    <t>do you desire the answer to that question?</t>
+    <t>SetTopic</t>
+  </si>
+  <si>
+    <t>SetPayment</t>
+  </si>
+  <si>
+    <t>{Amount} {Payment} will suffice</t>
+  </si>
+  <si>
+    <t>{Amount} {Payment} is the price</t>
+  </si>
+  <si>
+    <t>Test1_08</t>
+  </si>
+  <si>
+    <t>Seek your reward in the morning</t>
+  </si>
+  <si>
+    <t>Test2_1</t>
+  </si>
+  <si>
+    <t>DayExausted</t>
   </si>
 </sst>
 </file>
@@ -547,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165FA3C8-A4D7-491C-B60D-CA9B9E06CBE3}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,14 +547,14 @@
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" customWidth="1"/>
     <col min="15" max="15" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,251 +586,231 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="str">
+        <f>$A$7</f>
+        <v>Test1_07</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="str">
+        <f>$A$7</f>
+        <v>Test1_07</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="str">
+        <f>$A$7</f>
+        <v>Test1_07</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="str">
-        <f>A9</f>
-        <v>Test1_021</v>
-      </c>
-      <c r="H4" t="str">
-        <f>A10</f>
-        <v>Test1_022</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="str">
-        <f>$A$8</f>
-        <v>Test1_07</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="str">
-        <f>$A$8</f>
-        <v>Test1_07</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="str">
-        <f>$A$8</f>
-        <v>Test1_07</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="str">
+        <f>A7</f>
+        <v>Test1_07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="H8" t="s">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="str">
-        <f>$A$8</f>
-        <v>Test1_07</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="str">
-        <f>A8</f>
-        <v>Test1_07</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -886,10 +848,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,33 +859,33 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1191,16 +1153,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98FC212B-9056-4896-AFBB-7407AB275A44}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="740670c3-5ddc-4de0-a415-67ca36e0ce9e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b84d5890-a91a-48c6-834e-16c1483eadee"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b84d5890-a91a-48c6-834e-16c1483eadee"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="740670c3-5ddc-4de0-a415-67ca36e0ce9e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>